<commit_message>
Finish assesement of articles (319 articles reviewed; 112 applied multiverse-type analysis).
</commit_message>
<xml_diff>
--- a/articles_metadata.xlsx
+++ b/articles_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlenda1\Multiverse-type-Visualizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35DB1A4-D13C-494B-AE66-75CC3BB0E35D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00D1750-0B53-42D0-AA23-3A52D97917C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="980">
   <si>
     <t>title</t>
   </si>
@@ -2749,9 +2749,6 @@
     <t>http://www.psysci.org/CN/article/downloadArticleFile.do?attachType=PDF&amp;id=10313</t>
   </si>
   <si>
-    <t>https://www.nature.com/articles/s41562-016-0021%C3%82%C2%A0</t>
-  </si>
-  <si>
     <t>https://journals.sagepub.com/doi/abs/10.1177/1745691616658637</t>
   </si>
   <si>
@@ -2954,6 +2951,15 @@
   </si>
   <si>
     <t>page around 100</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41562-016-0021</t>
+  </si>
+  <si>
+    <t>mvs paper</t>
+  </si>
+  <si>
+    <t>metaanalysis</t>
   </si>
 </sst>
 </file>
@@ -3321,33 +3327,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="G258" sqref="G258"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="G270" sqref="G270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>971</v>
+      </c>
+      <c r="D1" t="s">
         <v>972</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>973</v>
-      </c>
-      <c r="E1" t="s">
-        <v>974</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -3373,10 +3379,10 @@
         <v>638</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G2" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3396,10 +3402,10 @@
         <v>639</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3419,10 +3425,10 @@
         <v>640</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G4" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3442,10 +3448,10 @@
         <v>641</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G5" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3465,10 +3471,10 @@
         <v>642</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3488,10 +3494,10 @@
         <v>643</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G7" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3511,10 +3517,10 @@
         <v>644</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G8" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3534,10 +3540,10 @@
         <v>645</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G9" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -3557,10 +3563,10 @@
         <v>646</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G10" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -3580,10 +3586,10 @@
         <v>647</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G11" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -3603,10 +3609,10 @@
         <v>648</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G12" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -3626,10 +3632,10 @@
         <v>649</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G13" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3649,10 +3655,10 @@
         <v>650</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G14" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3672,10 +3678,10 @@
         <v>651</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G15" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -3695,10 +3701,10 @@
         <v>652</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G16" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3718,10 +3724,10 @@
         <v>653</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G17" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3741,10 +3747,10 @@
         <v>654</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G18" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3764,10 +3770,10 @@
         <v>655</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G19" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3787,10 +3793,10 @@
         <v>656</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G20" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -3810,10 +3816,10 @@
         <v>657</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G21" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -3833,10 +3839,10 @@
         <v>658</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G22" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -3856,10 +3862,10 @@
         <v>659</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G23" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3879,10 +3885,10 @@
         <v>660</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G24" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3902,10 +3908,10 @@
         <v>661</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G25" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3925,10 +3931,10 @@
         <v>662</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G26" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -3948,10 +3954,10 @@
         <v>663</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G27" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -3971,10 +3977,10 @@
         <v>664</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G28" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -3994,10 +4000,10 @@
         <v>665</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G29" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4017,10 +4023,10 @@
         <v>666</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G30" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4040,10 +4046,10 @@
         <v>667</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G31" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4063,10 +4069,10 @@
         <v>668</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G32" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4086,10 +4092,10 @@
         <v>669</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G33" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4109,10 +4115,10 @@
         <v>670</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G34" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4132,10 +4138,10 @@
         <v>671</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G35" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4155,10 +4161,10 @@
         <v>672</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G36" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4178,10 +4184,10 @@
         <v>673</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G37" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4201,10 +4207,10 @@
         <v>674</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G38" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4224,10 +4230,10 @@
         <v>675</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G39" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4247,10 +4253,10 @@
         <v>676</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G40" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4270,10 +4276,10 @@
         <v>677</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G41" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4293,10 +4299,10 @@
         <v>678</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G42" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4316,10 +4322,10 @@
         <v>679</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G43" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4339,10 +4345,10 @@
         <v>680</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G44" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -4362,10 +4368,10 @@
         <v>681</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G45" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4385,10 +4391,10 @@
         <v>682</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G46" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -4408,10 +4414,10 @@
         <v>683</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G47" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4431,10 +4437,10 @@
         <v>684</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G48" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -4454,10 +4460,10 @@
         <v>685</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G49" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -4477,10 +4483,10 @@
         <v>686</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G50" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -4500,10 +4506,10 @@
         <v>687</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G51" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -4523,10 +4529,10 @@
         <v>688</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G52" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -4546,10 +4552,10 @@
         <v>689</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G53" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -4569,10 +4575,10 @@
         <v>690</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G54" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -4592,10 +4598,10 @@
         <v>691</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G55" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -4615,10 +4621,10 @@
         <v>692</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G56" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -4638,10 +4644,10 @@
         <v>693</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G57" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -4661,10 +4667,10 @@
         <v>694</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G58" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -4684,10 +4690,10 @@
         <v>695</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G59" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -4707,10 +4713,10 @@
         <v>696</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G60" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -4730,10 +4736,10 @@
         <v>697</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G61" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -4753,10 +4759,10 @@
         <v>698</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G62" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -4776,10 +4782,10 @@
         <v>699</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G63" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -4799,10 +4805,10 @@
         <v>700</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G64" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -4822,10 +4828,10 @@
         <v>701</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G65" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -4845,10 +4851,10 @@
         <v>702</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G66" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -4868,10 +4874,10 @@
         <v>703</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G67" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -4891,10 +4897,10 @@
         <v>704</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G68" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -4914,10 +4920,10 @@
         <v>705</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G69" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -4937,10 +4943,10 @@
         <v>706</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G70" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -4960,10 +4966,10 @@
         <v>707</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G71" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -4983,10 +4989,10 @@
         <v>708</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G72" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -5006,10 +5012,10 @@
         <v>709</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G73" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -5029,10 +5035,10 @@
         <v>710</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G74" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -5052,10 +5058,10 @@
         <v>711</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G75" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -5075,10 +5081,10 @@
         <v>712</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G76" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -5098,10 +5104,10 @@
         <v>713</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G77" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -5121,10 +5127,10 @@
         <v>714</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G78" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -5144,10 +5150,10 @@
         <v>715</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G79" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -5167,10 +5173,10 @@
         <v>716</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G80" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -5190,10 +5196,10 @@
         <v>717</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G81" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -5213,10 +5219,10 @@
         <v>718</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G82" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -5236,10 +5242,10 @@
         <v>719</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G83" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -5259,10 +5265,10 @@
         <v>720</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G84" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -5282,10 +5288,10 @@
         <v>721</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G85" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -5305,10 +5311,10 @@
         <v>722</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G86" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -5328,10 +5334,10 @@
         <v>723</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G87" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -5351,10 +5357,10 @@
         <v>724</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G88" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -5374,10 +5380,10 @@
         <v>725</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G89" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -5397,10 +5403,10 @@
         <v>726</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G90" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -5420,10 +5426,10 @@
         <v>727</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G91" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -5443,10 +5449,10 @@
         <v>728</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G92" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -5466,10 +5472,10 @@
         <v>729</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G93" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -5489,10 +5495,10 @@
         <v>730</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G94" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -5512,10 +5518,10 @@
         <v>731</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G95" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -5535,10 +5541,10 @@
         <v>732</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G96" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -5558,10 +5564,10 @@
         <v>733</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G97" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -5581,10 +5587,10 @@
         <v>734</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G98" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -5604,10 +5610,10 @@
         <v>735</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G99" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -5627,10 +5633,10 @@
         <v>736</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G100" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -5650,10 +5656,10 @@
         <v>737</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G101" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -5673,10 +5679,10 @@
         <v>738</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G102" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -5696,10 +5702,10 @@
         <v>739</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G103" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -5719,10 +5725,10 @@
         <v>740</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G104" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -5742,10 +5748,10 @@
         <v>741</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G105" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -5765,10 +5771,10 @@
         <v>742</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G106" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -5788,10 +5794,10 @@
         <v>743</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G107" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -5811,10 +5817,10 @@
         <v>744</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G108" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -5834,10 +5840,10 @@
         <v>745</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G109" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -5857,10 +5863,10 @@
         <v>746</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G110" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -5880,10 +5886,10 @@
         <v>747</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G111" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -5903,10 +5909,10 @@
         <v>748</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G112" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -5926,10 +5932,10 @@
         <v>749</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G113" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -5949,10 +5955,10 @@
         <v>750</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G114" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -5972,10 +5978,10 @@
         <v>751</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G115" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -5995,10 +6001,10 @@
         <v>752</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G116" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -6018,10 +6024,10 @@
         <v>753</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G117" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -6041,10 +6047,10 @@
         <v>754</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G118" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -6064,10 +6070,10 @@
         <v>755</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G119" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -6087,10 +6093,10 @@
         <v>756</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G120" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -6110,10 +6116,10 @@
         <v>757</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G121" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -6133,10 +6139,10 @@
         <v>758</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G122" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -6156,10 +6162,10 @@
         <v>759</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G123" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -6179,10 +6185,10 @@
         <v>760</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G124" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -6202,10 +6208,10 @@
         <v>761</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G125" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -6225,10 +6231,10 @@
         <v>762</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G126" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
@@ -6248,10 +6254,10 @@
         <v>763</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G127" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
@@ -6271,10 +6277,10 @@
         <v>764</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G128" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -6294,10 +6300,10 @@
         <v>765</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G129" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
@@ -6317,10 +6323,10 @@
         <v>766</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G130" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -6340,10 +6346,10 @@
         <v>767</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G131" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -6363,10 +6369,10 @@
         <v>768</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G132" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -6386,10 +6392,10 @@
         <v>769</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G133" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -6409,10 +6415,10 @@
         <v>770</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G134" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -6432,10 +6438,10 @@
         <v>771</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G135" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -6455,10 +6461,10 @@
         <v>772</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G136" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -6478,10 +6484,10 @@
         <v>773</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G137" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -6501,10 +6507,10 @@
         <v>774</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G138" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -6524,10 +6530,10 @@
         <v>775</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G139" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -6547,10 +6553,10 @@
         <v>776</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G140" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -6570,10 +6576,10 @@
         <v>777</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G141" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -6593,10 +6599,10 @@
         <v>778</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G142" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -6616,10 +6622,10 @@
         <v>779</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G143" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -6639,10 +6645,10 @@
         <v>780</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G144" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -6662,10 +6668,10 @@
         <v>781</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G145" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -6685,10 +6691,10 @@
         <v>782</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G146" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -6708,10 +6714,10 @@
         <v>783</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G147" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -6731,10 +6737,10 @@
         <v>784</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G148" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -6754,10 +6760,10 @@
         <v>785</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G149" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -6777,10 +6783,10 @@
         <v>786</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G150" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -6800,10 +6806,10 @@
         <v>787</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G151" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -6823,10 +6829,10 @@
         <v>788</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G152" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -6846,10 +6852,10 @@
         <v>789</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G153" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -6869,10 +6875,10 @@
         <v>790</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G154" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -6892,10 +6898,10 @@
         <v>791</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G155" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -6915,10 +6921,10 @@
         <v>792</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G156" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -6938,10 +6944,10 @@
         <v>793</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G157" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -6961,10 +6967,10 @@
         <v>794</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G158" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -6984,10 +6990,10 @@
         <v>795</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G159" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -7007,10 +7013,10 @@
         <v>796</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G160" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -7030,10 +7036,10 @@
         <v>797</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G161" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -7053,10 +7059,10 @@
         <v>798</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G162" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -7076,10 +7082,10 @@
         <v>799</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G163" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -7099,10 +7105,10 @@
         <v>800</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G164" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -7122,10 +7128,10 @@
         <v>801</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G165" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -7145,10 +7151,10 @@
         <v>802</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G166" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -7168,10 +7174,10 @@
         <v>803</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G167" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -7191,10 +7197,10 @@
         <v>804</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G168" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -7214,10 +7220,10 @@
         <v>805</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G169" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -7237,10 +7243,10 @@
         <v>806</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G170" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -7260,10 +7266,10 @@
         <v>807</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G171" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -7283,10 +7289,10 @@
         <v>808</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G172" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -7306,10 +7312,10 @@
         <v>809</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G173" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -7329,10 +7335,10 @@
         <v>810</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G174" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -7352,10 +7358,10 @@
         <v>811</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G175" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -7375,10 +7381,10 @@
         <v>812</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G176" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -7398,10 +7404,10 @@
         <v>813</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G177" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -7421,10 +7427,10 @@
         <v>814</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G178" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
@@ -7444,10 +7450,10 @@
         <v>815</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G179" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -7467,10 +7473,10 @@
         <v>816</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G180" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -7490,10 +7496,10 @@
         <v>817</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G181" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -7513,10 +7519,10 @@
         <v>818</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G182" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
@@ -7536,10 +7542,10 @@
         <v>819</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G183" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
@@ -7559,10 +7565,10 @@
         <v>820</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G184" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
@@ -7582,10 +7588,10 @@
         <v>821</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G185" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
@@ -7605,10 +7611,10 @@
         <v>822</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G186" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -7628,10 +7634,10 @@
         <v>823</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G187" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -7651,10 +7657,10 @@
         <v>824</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G188" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -7674,10 +7680,10 @@
         <v>825</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G189" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -7697,10 +7703,10 @@
         <v>826</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G190" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -7720,10 +7726,10 @@
         <v>827</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G191" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -7743,10 +7749,10 @@
         <v>828</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G192" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -7766,10 +7772,10 @@
         <v>829</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G193" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -7789,10 +7795,10 @@
         <v>830</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G194" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -7812,10 +7818,10 @@
         <v>831</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G195" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -7835,10 +7841,10 @@
         <v>832</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G196" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
@@ -7858,10 +7864,10 @@
         <v>833</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G197" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -7881,10 +7887,10 @@
         <v>834</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G198" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -7904,10 +7910,10 @@
         <v>835</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G199" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -7927,10 +7933,10 @@
         <v>836</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G200" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -7950,10 +7956,10 @@
         <v>837</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G201" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
@@ -7973,10 +7979,10 @@
         <v>838</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G202" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -7996,10 +8002,10 @@
         <v>839</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G203" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
@@ -8019,10 +8025,10 @@
         <v>840</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G204" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
@@ -8042,10 +8048,10 @@
         <v>841</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G205" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
@@ -8065,10 +8071,10 @@
         <v>842</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G206" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -8088,10 +8094,10 @@
         <v>843</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G207" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
@@ -8111,10 +8117,10 @@
         <v>844</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G208" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
@@ -8134,10 +8140,10 @@
         <v>845</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G209" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
@@ -8157,10 +8163,10 @@
         <v>846</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G210" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -8180,10 +8186,10 @@
         <v>847</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G211" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
@@ -8203,10 +8209,10 @@
         <v>848</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G212" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -8226,10 +8232,10 @@
         <v>849</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G213" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -8252,7 +8258,7 @@
         <v>0</v>
       </c>
       <c r="G214" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -8275,7 +8281,7 @@
         <v>0</v>
       </c>
       <c r="G215" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -8298,7 +8304,7 @@
         <v>0</v>
       </c>
       <c r="G216" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -8321,7 +8327,7 @@
         <v>0</v>
       </c>
       <c r="G217" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -8344,7 +8350,7 @@
         <v>1</v>
       </c>
       <c r="G218" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -8367,7 +8373,7 @@
         <v>0</v>
       </c>
       <c r="G219" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -8390,7 +8396,7 @@
         <v>0</v>
       </c>
       <c r="G220" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -8413,7 +8419,7 @@
         <v>0</v>
       </c>
       <c r="G221" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
@@ -8436,7 +8442,7 @@
         <v>0</v>
       </c>
       <c r="G222" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -8459,7 +8465,7 @@
         <v>0</v>
       </c>
       <c r="G223" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -8482,7 +8488,7 @@
         <v>0</v>
       </c>
       <c r="G224" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -8505,7 +8511,7 @@
         <v>0</v>
       </c>
       <c r="G225" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -8528,7 +8534,7 @@
         <v>1</v>
       </c>
       <c r="G226" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -8551,7 +8557,7 @@
         <v>0</v>
       </c>
       <c r="G227" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -8574,7 +8580,7 @@
         <v>0</v>
       </c>
       <c r="G228" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -8597,7 +8603,7 @@
         <v>1</v>
       </c>
       <c r="G229" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -8640,7 +8646,7 @@
         <v>0</v>
       </c>
       <c r="G231" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -8663,7 +8669,7 @@
         <v>0</v>
       </c>
       <c r="G232" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -8686,7 +8692,7 @@
         <v>0</v>
       </c>
       <c r="G233" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -8709,7 +8715,7 @@
         <v>1</v>
       </c>
       <c r="G234" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -8732,7 +8738,7 @@
         <v>1</v>
       </c>
       <c r="G235" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -8755,7 +8761,7 @@
         <v>0</v>
       </c>
       <c r="G236" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -8778,7 +8784,7 @@
         <v>1</v>
       </c>
       <c r="G237" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -8801,7 +8807,7 @@
         <v>0</v>
       </c>
       <c r="G238" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -8824,7 +8830,7 @@
         <v>0</v>
       </c>
       <c r="G239" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -8847,7 +8853,7 @@
         <v>0</v>
       </c>
       <c r="G240" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -8870,7 +8876,7 @@
         <v>1</v>
       </c>
       <c r="G241" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -8893,7 +8899,7 @@
         <v>0</v>
       </c>
       <c r="G242" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -8916,7 +8922,7 @@
         <v>1</v>
       </c>
       <c r="G243" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -8939,7 +8945,7 @@
         <v>0</v>
       </c>
       <c r="G244" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -8962,7 +8968,7 @@
         <v>0</v>
       </c>
       <c r="G245" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -8985,7 +8991,7 @@
         <v>0</v>
       </c>
       <c r="G246" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -9008,7 +9014,7 @@
         <v>0</v>
       </c>
       <c r="G247" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -9031,7 +9037,7 @@
         <v>1</v>
       </c>
       <c r="G248" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -9074,7 +9080,7 @@
         <v>0</v>
       </c>
       <c r="G250" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -9090,14 +9096,14 @@
       <c r="D251" t="s">
         <v>632</v>
       </c>
-      <c r="E251" t="s">
+      <c r="E251" s="2" t="s">
         <v>887</v>
       </c>
-      <c r="F251" s="1" t="s">
-        <v>960</v>
+      <c r="F251" s="1">
+        <v>0</v>
       </c>
       <c r="G251" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -9113,14 +9119,14 @@
       <c r="D252" t="s">
         <v>632</v>
       </c>
-      <c r="E252" t="s">
+      <c r="E252" s="2" t="s">
         <v>888</v>
       </c>
-      <c r="F252" s="1" t="s">
-        <v>960</v>
+      <c r="F252" s="1">
+        <v>0</v>
       </c>
       <c r="G252" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -9136,14 +9142,14 @@
       <c r="D253" t="s">
         <v>631</v>
       </c>
-      <c r="E253" t="s">
+      <c r="E253" s="2" t="s">
         <v>889</v>
       </c>
-      <c r="F253" s="1" t="s">
-        <v>960</v>
+      <c r="F253" s="1">
+        <v>0</v>
       </c>
       <c r="G253" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -9159,14 +9165,14 @@
       <c r="D254" t="s">
         <v>632</v>
       </c>
-      <c r="E254" t="s">
+      <c r="E254" s="2" t="s">
         <v>890</v>
       </c>
-      <c r="F254" s="1" t="s">
-        <v>960</v>
+      <c r="F254" s="1">
+        <v>1</v>
       </c>
       <c r="G254" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -9182,14 +9188,14 @@
       <c r="D255" t="s">
         <v>632</v>
       </c>
-      <c r="E255" t="s">
+      <c r="E255" s="2" t="s">
         <v>891</v>
       </c>
-      <c r="F255" s="1" t="s">
-        <v>960</v>
+      <c r="F255" s="1">
+        <v>0</v>
       </c>
       <c r="G255" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -9205,14 +9211,14 @@
       <c r="D256" t="s">
         <v>632</v>
       </c>
-      <c r="E256" t="s">
+      <c r="E256" s="2" t="s">
         <v>892</v>
       </c>
-      <c r="F256" s="1" t="s">
-        <v>960</v>
+      <c r="F256" s="1">
+        <v>0</v>
       </c>
       <c r="G256" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -9228,14 +9234,14 @@
       <c r="D257" t="s">
         <v>632</v>
       </c>
-      <c r="E257" t="s">
+      <c r="E257" s="2" t="s">
         <v>893</v>
       </c>
-      <c r="F257" s="1" t="s">
-        <v>960</v>
+      <c r="F257" s="1">
+        <v>1</v>
       </c>
       <c r="G257" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -9254,11 +9260,11 @@
       <c r="E258" t="s">
         <v>894</v>
       </c>
-      <c r="F258" s="1" t="s">
-        <v>960</v>
+      <c r="F258" s="1">
+        <v>0</v>
       </c>
       <c r="G258" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -9274,14 +9280,14 @@
       <c r="D259" t="s">
         <v>632</v>
       </c>
-      <c r="E259" t="s">
+      <c r="E259" s="2" t="s">
         <v>895</v>
       </c>
-      <c r="F259" s="1" t="s">
-        <v>960</v>
+      <c r="F259" s="1">
+        <v>0</v>
       </c>
       <c r="G259" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -9297,14 +9303,14 @@
       <c r="D260" t="s">
         <v>632</v>
       </c>
-      <c r="E260" t="s">
+      <c r="E260" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="F260" s="1" t="s">
-        <v>960</v>
+      <c r="F260" s="1">
+        <v>0</v>
       </c>
       <c r="G260" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -9320,14 +9326,14 @@
       <c r="D261" t="s">
         <v>632</v>
       </c>
-      <c r="E261" t="s">
+      <c r="E261" s="2" t="s">
         <v>897</v>
       </c>
-      <c r="F261" s="1" t="s">
-        <v>960</v>
+      <c r="F261" s="1">
+        <v>0</v>
       </c>
       <c r="G261" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -9343,14 +9349,14 @@
       <c r="D262" t="s">
         <v>632</v>
       </c>
-      <c r="E262" t="s">
+      <c r="E262" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="F262" s="1" t="s">
-        <v>960</v>
+      <c r="F262" s="1">
+        <v>0</v>
       </c>
       <c r="G262" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
@@ -9366,14 +9372,14 @@
       <c r="D263" t="s">
         <v>632</v>
       </c>
-      <c r="E263" t="s">
+      <c r="E263" s="2" t="s">
         <v>899</v>
       </c>
-      <c r="F263" s="1" t="s">
-        <v>960</v>
+      <c r="F263" s="1">
+        <v>0</v>
       </c>
       <c r="G263" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
@@ -9389,14 +9395,14 @@
       <c r="D264" t="s">
         <v>632</v>
       </c>
-      <c r="E264" t="s">
+      <c r="E264" s="2" t="s">
         <v>900</v>
       </c>
-      <c r="F264" s="1" t="s">
-        <v>960</v>
+      <c r="F264" s="1">
+        <v>0</v>
       </c>
       <c r="G264" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -9412,14 +9418,14 @@
       <c r="D265" t="s">
         <v>632</v>
       </c>
-      <c r="E265" t="s">
+      <c r="E265" s="2" t="s">
         <v>901</v>
       </c>
-      <c r="F265" s="1" t="s">
-        <v>960</v>
+      <c r="F265" s="1">
+        <v>0</v>
       </c>
       <c r="G265" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
@@ -9435,14 +9441,14 @@
       <c r="D266" t="s">
         <v>632</v>
       </c>
-      <c r="E266" t="s">
+      <c r="E266" s="2" t="s">
         <v>902</v>
       </c>
-      <c r="F266" s="1" t="s">
-        <v>960</v>
+      <c r="F266" s="1">
+        <v>0</v>
       </c>
       <c r="G266" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
@@ -9458,14 +9464,14 @@
       <c r="D267" t="s">
         <v>632</v>
       </c>
-      <c r="E267" t="s">
+      <c r="E267" s="2" t="s">
         <v>903</v>
       </c>
-      <c r="F267" s="1" t="s">
-        <v>960</v>
+      <c r="F267" s="1">
+        <v>0</v>
       </c>
       <c r="G267" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
@@ -9481,14 +9487,14 @@
       <c r="D268" t="s">
         <v>632</v>
       </c>
-      <c r="E268" t="s">
+      <c r="E268" s="2" t="s">
         <v>904</v>
       </c>
-      <c r="F268" s="1" t="s">
-        <v>960</v>
+      <c r="F268" s="1">
+        <v>0</v>
       </c>
       <c r="G268" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
@@ -9504,14 +9510,14 @@
       <c r="D269" t="s">
         <v>632</v>
       </c>
-      <c r="E269" t="s">
+      <c r="E269" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="F269" s="1" t="s">
-        <v>960</v>
+      <c r="F269" s="1">
+        <v>1</v>
       </c>
       <c r="G269" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
@@ -9530,11 +9536,11 @@
       <c r="E270" t="s">
         <v>906</v>
       </c>
-      <c r="F270" s="1" t="s">
-        <v>960</v>
+      <c r="F270" s="1">
+        <v>0</v>
       </c>
       <c r="G270" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
@@ -9553,11 +9559,11 @@
       <c r="E271" t="s">
         <v>907</v>
       </c>
-      <c r="F271" s="1" t="s">
-        <v>960</v>
+      <c r="F271" s="1">
+        <v>0</v>
       </c>
       <c r="G271" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
@@ -9576,11 +9582,11 @@
       <c r="E272" t="s">
         <v>908</v>
       </c>
-      <c r="F272" s="1" t="s">
-        <v>960</v>
+      <c r="F272" s="1">
+        <v>0</v>
       </c>
       <c r="G272" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.3">
@@ -9596,14 +9602,14 @@
       <c r="D273" t="s">
         <v>630</v>
       </c>
-      <c r="E273" t="s">
-        <v>909</v>
-      </c>
-      <c r="F273" s="1" t="s">
-        <v>960</v>
+      <c r="E273" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="F273" s="1">
+        <v>0</v>
       </c>
       <c r="G273" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
@@ -9620,13 +9626,13 @@
         <v>629</v>
       </c>
       <c r="E274" t="s">
-        <v>910</v>
-      </c>
-      <c r="F274" s="1" t="s">
-        <v>960</v>
+        <v>909</v>
+      </c>
+      <c r="F274" s="1">
+        <v>1</v>
       </c>
       <c r="G274" t="s">
-        <v>960</v>
+        <v>978</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
@@ -9642,14 +9648,14 @@
       <c r="D275" t="s">
         <v>629</v>
       </c>
-      <c r="E275" t="s">
-        <v>911</v>
-      </c>
-      <c r="F275" s="1" t="s">
-        <v>960</v>
+      <c r="E275" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="F275" s="1">
+        <v>1</v>
       </c>
       <c r="G275" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
@@ -9665,14 +9671,14 @@
       <c r="D276" t="s">
         <v>630</v>
       </c>
-      <c r="E276" t="s">
-        <v>912</v>
-      </c>
-      <c r="F276" s="1" t="s">
-        <v>960</v>
+      <c r="E276" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="F276" s="1">
+        <v>0</v>
       </c>
       <c r="G276" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
@@ -9688,14 +9694,14 @@
       <c r="D277" t="s">
         <v>629</v>
       </c>
-      <c r="E277" t="s">
-        <v>913</v>
-      </c>
-      <c r="F277" s="1" t="s">
-        <v>960</v>
+      <c r="E277" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="F277" s="1">
+        <v>1</v>
       </c>
       <c r="G277" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
@@ -9711,14 +9717,14 @@
       <c r="D278" t="s">
         <v>630</v>
       </c>
-      <c r="E278" t="s">
-        <v>914</v>
-      </c>
-      <c r="F278" s="1" t="s">
-        <v>960</v>
+      <c r="E278" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="F278" s="1">
+        <v>0</v>
       </c>
       <c r="G278" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
@@ -9734,14 +9740,14 @@
       <c r="D279" t="s">
         <v>629</v>
       </c>
-      <c r="E279" t="s">
-        <v>915</v>
-      </c>
-      <c r="F279" s="1" t="s">
-        <v>960</v>
+      <c r="E279" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="F279" s="1">
+        <v>0</v>
       </c>
       <c r="G279" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.3">
@@ -9757,14 +9763,14 @@
       <c r="D280" t="s">
         <v>630</v>
       </c>
-      <c r="E280" t="s">
-        <v>916</v>
-      </c>
-      <c r="F280" s="1" t="s">
-        <v>960</v>
+      <c r="E280" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="F280" s="1">
+        <v>1</v>
       </c>
       <c r="G280" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
@@ -9780,14 +9786,14 @@
       <c r="D281" t="s">
         <v>630</v>
       </c>
-      <c r="E281" t="s">
-        <v>917</v>
-      </c>
-      <c r="F281" s="1" t="s">
-        <v>960</v>
+      <c r="E281" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="F281" s="1">
+        <v>0</v>
       </c>
       <c r="G281" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
@@ -9803,14 +9809,14 @@
       <c r="D282" t="s">
         <v>630</v>
       </c>
-      <c r="E282" t="s">
-        <v>918</v>
-      </c>
-      <c r="F282" s="1" t="s">
-        <v>960</v>
+      <c r="E282" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="F282" s="1">
+        <v>0</v>
       </c>
       <c r="G282" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.3">
@@ -9826,14 +9832,14 @@
       <c r="D283" t="s">
         <v>630</v>
       </c>
-      <c r="E283" t="s">
-        <v>919</v>
-      </c>
-      <c r="F283" s="1" t="s">
-        <v>960</v>
+      <c r="E283" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="F283" s="1">
+        <v>1</v>
       </c>
       <c r="G283" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
@@ -9849,14 +9855,14 @@
       <c r="D284" t="s">
         <v>629</v>
       </c>
-      <c r="E284" t="s">
-        <v>920</v>
-      </c>
-      <c r="F284" s="1" t="s">
-        <v>960</v>
+      <c r="E284" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="F284" s="1">
+        <v>1</v>
       </c>
       <c r="G284" t="s">
-        <v>960</v>
+        <v>979</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.3">
@@ -9872,14 +9878,14 @@
       <c r="D285" t="s">
         <v>630</v>
       </c>
-      <c r="E285" t="s">
-        <v>921</v>
-      </c>
-      <c r="F285" s="1" t="s">
-        <v>960</v>
+      <c r="E285" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="F285" s="1">
+        <v>0</v>
       </c>
       <c r="G285" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.3">
@@ -9895,14 +9901,14 @@
       <c r="D286" t="s">
         <v>631</v>
       </c>
-      <c r="E286" t="s">
-        <v>922</v>
-      </c>
-      <c r="F286" s="1" t="s">
-        <v>960</v>
+      <c r="E286" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="F286" s="1">
+        <v>1</v>
       </c>
       <c r="G286" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.3">
@@ -9918,14 +9924,14 @@
       <c r="D287" t="s">
         <v>629</v>
       </c>
-      <c r="E287" t="s">
-        <v>923</v>
-      </c>
-      <c r="F287" s="1" t="s">
-        <v>960</v>
+      <c r="E287" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="F287" s="1">
+        <v>1</v>
       </c>
       <c r="G287" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.3">
@@ -9941,14 +9947,14 @@
       <c r="D288" t="s">
         <v>632</v>
       </c>
-      <c r="E288" t="s">
-        <v>924</v>
-      </c>
-      <c r="F288" s="1" t="s">
-        <v>960</v>
+      <c r="E288" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="F288" s="1">
+        <v>0</v>
       </c>
       <c r="G288" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.3">
@@ -9964,14 +9970,14 @@
       <c r="D289" t="s">
         <v>631</v>
       </c>
-      <c r="E289" t="s">
-        <v>925</v>
-      </c>
-      <c r="F289" s="1" t="s">
-        <v>960</v>
+      <c r="E289" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="F289" s="1">
+        <v>0</v>
       </c>
       <c r="G289" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.3">
@@ -9987,14 +9993,14 @@
       <c r="D290" t="s">
         <v>631</v>
       </c>
-      <c r="E290" t="s">
-        <v>926</v>
-      </c>
-      <c r="F290" s="1" t="s">
-        <v>960</v>
+      <c r="E290" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="F290" s="1">
+        <v>0</v>
       </c>
       <c r="G290" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.3">
@@ -10010,14 +10016,14 @@
       <c r="D291" t="s">
         <v>630</v>
       </c>
-      <c r="E291" t="s">
-        <v>927</v>
-      </c>
-      <c r="F291" s="1" t="s">
-        <v>960</v>
+      <c r="E291" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="F291" s="1">
+        <v>0</v>
       </c>
       <c r="G291" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.3">
@@ -10033,14 +10039,14 @@
       <c r="D292" t="s">
         <v>630</v>
       </c>
-      <c r="E292" t="s">
-        <v>928</v>
-      </c>
-      <c r="F292" s="1" t="s">
-        <v>960</v>
+      <c r="E292" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="F292" s="1">
+        <v>0</v>
       </c>
       <c r="G292" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.3">
@@ -10056,14 +10062,14 @@
       <c r="D293" t="s">
         <v>631</v>
       </c>
-      <c r="E293" t="s">
-        <v>929</v>
-      </c>
-      <c r="F293" s="1" t="s">
-        <v>960</v>
+      <c r="E293" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="F293" s="1">
+        <v>0</v>
       </c>
       <c r="G293" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.3">
@@ -10079,14 +10085,14 @@
       <c r="D294" t="s">
         <v>631</v>
       </c>
-      <c r="E294" t="s">
-        <v>930</v>
-      </c>
-      <c r="F294" s="1" t="s">
-        <v>960</v>
+      <c r="E294" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="F294" s="1">
+        <v>1</v>
       </c>
       <c r="G294" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.3">
@@ -10102,14 +10108,14 @@
       <c r="D295" t="s">
         <v>630</v>
       </c>
-      <c r="E295" t="s">
-        <v>931</v>
-      </c>
-      <c r="F295" s="1" t="s">
-        <v>960</v>
+      <c r="E295" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="F295" s="1">
+        <v>1</v>
       </c>
       <c r="G295" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.3">
@@ -10125,14 +10131,14 @@
       <c r="D296" t="s">
         <v>629</v>
       </c>
-      <c r="E296" t="s">
-        <v>932</v>
-      </c>
-      <c r="F296" s="1" t="s">
-        <v>960</v>
+      <c r="E296" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="F296" s="1">
+        <v>0</v>
       </c>
       <c r="G296" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.3">
@@ -10148,14 +10154,14 @@
       <c r="D297" t="s">
         <v>629</v>
       </c>
-      <c r="E297" t="s">
-        <v>933</v>
-      </c>
-      <c r="F297" s="1" t="s">
-        <v>960</v>
+      <c r="E297" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="F297" s="1">
+        <v>1</v>
       </c>
       <c r="G297" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.3">
@@ -10171,14 +10177,14 @@
       <c r="D298" t="s">
         <v>630</v>
       </c>
-      <c r="E298" t="s">
-        <v>934</v>
-      </c>
-      <c r="F298" s="1" t="s">
-        <v>960</v>
+      <c r="E298" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="F298" s="1">
+        <v>1</v>
       </c>
       <c r="G298" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.3">
@@ -10194,14 +10200,14 @@
       <c r="D299" t="s">
         <v>632</v>
       </c>
-      <c r="E299" t="s">
-        <v>935</v>
-      </c>
-      <c r="F299" s="1" t="s">
-        <v>960</v>
+      <c r="E299" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="F299" s="1">
+        <v>0</v>
       </c>
       <c r="G299" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.3">
@@ -10217,14 +10223,14 @@
       <c r="D300" t="s">
         <v>632</v>
       </c>
-      <c r="E300" t="s">
-        <v>936</v>
-      </c>
-      <c r="F300" s="1" t="s">
-        <v>960</v>
+      <c r="E300" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="F300" s="1">
+        <v>1</v>
       </c>
       <c r="G300" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.3">
@@ -10240,14 +10246,14 @@
       <c r="D301" t="s">
         <v>630</v>
       </c>
-      <c r="E301" t="s">
-        <v>937</v>
-      </c>
-      <c r="F301" s="1" t="s">
-        <v>960</v>
+      <c r="E301" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="F301" s="1">
+        <v>0</v>
       </c>
       <c r="G301" t="s">
-        <v>960</v>
+        <v>968</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.3">
@@ -10263,14 +10269,14 @@
       <c r="D302" t="s">
         <v>632</v>
       </c>
-      <c r="E302" t="s">
-        <v>938</v>
-      </c>
-      <c r="F302" s="1" t="s">
-        <v>960</v>
+      <c r="E302" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="F302" s="1">
+        <v>0</v>
       </c>
       <c r="G302" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.3">
@@ -10287,13 +10293,13 @@
         <v>629</v>
       </c>
       <c r="E303" t="s">
-        <v>939</v>
-      </c>
-      <c r="F303" s="1" t="s">
-        <v>960</v>
+        <v>938</v>
+      </c>
+      <c r="F303" s="1">
+        <v>1</v>
       </c>
       <c r="G303" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.3">
@@ -10309,14 +10315,14 @@
       <c r="D304" t="s">
         <v>629</v>
       </c>
-      <c r="E304" t="s">
-        <v>940</v>
-      </c>
-      <c r="F304" s="1" t="s">
-        <v>960</v>
+      <c r="E304" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="F304" s="1">
+        <v>0</v>
       </c>
       <c r="G304" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.3">
@@ -10332,14 +10338,14 @@
       <c r="D305" t="s">
         <v>632</v>
       </c>
-      <c r="E305" t="s">
-        <v>941</v>
-      </c>
-      <c r="F305" s="1" t="s">
-        <v>960</v>
+      <c r="E305" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="F305" s="1">
+        <v>0</v>
       </c>
       <c r="G305" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.3">
@@ -10355,14 +10361,14 @@
       <c r="D306" t="s">
         <v>631</v>
       </c>
-      <c r="E306" t="s">
-        <v>942</v>
-      </c>
-      <c r="F306" s="1" t="s">
-        <v>960</v>
+      <c r="E306" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="F306" s="1">
+        <v>0</v>
       </c>
       <c r="G306" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.3">
@@ -10378,14 +10384,14 @@
       <c r="D307" t="s">
         <v>632</v>
       </c>
-      <c r="E307" t="s">
-        <v>943</v>
-      </c>
-      <c r="F307" s="1" t="s">
-        <v>960</v>
+      <c r="E307" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="F307" s="1">
+        <v>0</v>
       </c>
       <c r="G307" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.3">
@@ -10401,14 +10407,14 @@
       <c r="D308" t="s">
         <v>632</v>
       </c>
-      <c r="E308" t="s">
-        <v>944</v>
-      </c>
-      <c r="F308" s="1" t="s">
-        <v>960</v>
+      <c r="E308" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F308" s="1">
+        <v>0</v>
       </c>
       <c r="G308" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.3">
@@ -10424,14 +10430,14 @@
       <c r="D309" t="s">
         <v>632</v>
       </c>
-      <c r="E309" t="s">
-        <v>945</v>
-      </c>
-      <c r="F309" s="1" t="s">
-        <v>960</v>
+      <c r="E309" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="F309" s="1">
+        <v>0</v>
       </c>
       <c r="G309" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.3">
@@ -10447,14 +10453,14 @@
       <c r="D310" t="s">
         <v>631</v>
       </c>
-      <c r="E310" t="s">
-        <v>946</v>
-      </c>
-      <c r="F310" s="1" t="s">
-        <v>960</v>
+      <c r="E310" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="F310" s="1">
+        <v>0</v>
       </c>
       <c r="G310" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.3">
@@ -10470,14 +10476,14 @@
       <c r="D311" t="s">
         <v>632</v>
       </c>
-      <c r="E311" t="s">
-        <v>947</v>
-      </c>
-      <c r="F311" s="1" t="s">
-        <v>960</v>
+      <c r="E311" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="F311" s="1">
+        <v>0</v>
       </c>
       <c r="G311" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.3">
@@ -10494,13 +10500,13 @@
         <v>632</v>
       </c>
       <c r="E312" t="s">
-        <v>948</v>
-      </c>
-      <c r="F312" s="1" t="s">
-        <v>960</v>
+        <v>947</v>
+      </c>
+      <c r="F312" s="1">
+        <v>0</v>
       </c>
       <c r="G312" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.3">
@@ -10516,14 +10522,14 @@
       <c r="D313" t="s">
         <v>632</v>
       </c>
-      <c r="E313" t="s">
-        <v>949</v>
-      </c>
-      <c r="F313" s="1" t="s">
-        <v>960</v>
+      <c r="E313" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="F313" s="1">
+        <v>0</v>
       </c>
       <c r="G313" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.3">
@@ -10539,14 +10545,14 @@
       <c r="D314" t="s">
         <v>631</v>
       </c>
-      <c r="E314" t="s">
-        <v>950</v>
-      </c>
-      <c r="F314" s="1" t="s">
-        <v>960</v>
+      <c r="E314" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="F314" s="1">
+        <v>0</v>
       </c>
       <c r="G314" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.3">
@@ -10562,14 +10568,14 @@
       <c r="D315" t="s">
         <v>632</v>
       </c>
-      <c r="E315" t="s">
-        <v>951</v>
-      </c>
-      <c r="F315" s="1" t="s">
-        <v>960</v>
+      <c r="E315" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="F315" s="1">
+        <v>1</v>
       </c>
       <c r="G315" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.3">
@@ -10585,14 +10591,14 @@
       <c r="D316" t="s">
         <v>632</v>
       </c>
-      <c r="E316" t="s">
-        <v>952</v>
-      </c>
-      <c r="F316" s="1" t="s">
-        <v>960</v>
+      <c r="E316" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="F316" s="1">
+        <v>0</v>
       </c>
       <c r="G316" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.3">
@@ -10608,14 +10614,14 @@
       <c r="D317" t="s">
         <v>630</v>
       </c>
-      <c r="E317" t="s">
-        <v>953</v>
-      </c>
-      <c r="F317" s="1" t="s">
-        <v>960</v>
+      <c r="E317" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="F317" s="1">
+        <v>1</v>
       </c>
       <c r="G317" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
@@ -10631,14 +10637,14 @@
       <c r="D318" t="s">
         <v>631</v>
       </c>
-      <c r="E318" t="s">
-        <v>954</v>
-      </c>
-      <c r="F318" s="1" t="s">
-        <v>960</v>
+      <c r="E318" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="F318" s="1">
+        <v>0</v>
       </c>
       <c r="G318" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.3">
@@ -10654,14 +10660,14 @@
       <c r="D319" t="s">
         <v>632</v>
       </c>
-      <c r="E319" t="s">
-        <v>955</v>
-      </c>
-      <c r="F319" s="1" t="s">
-        <v>960</v>
+      <c r="E319" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="F319" s="1">
+        <v>1</v>
       </c>
       <c r="G319" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.3">
@@ -10678,13 +10684,13 @@
         <v>633</v>
       </c>
       <c r="E320" t="s">
-        <v>956</v>
-      </c>
-      <c r="F320" s="1" t="s">
-        <v>960</v>
+        <v>955</v>
+      </c>
+      <c r="F320" s="1">
+        <v>0</v>
       </c>
       <c r="G320" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
     </row>
   </sheetData>
@@ -10726,6 +10732,68 @@
     <hyperlink ref="E248" r:id="rId35" xr:uid="{DE62CE30-2474-4476-8D3B-CA434C457E3B}"/>
     <hyperlink ref="E249" r:id="rId36" xr:uid="{BEAAC372-AA6F-42E0-B69A-A80C9BCBF1F4}"/>
     <hyperlink ref="E250" r:id="rId37" xr:uid="{AA5C2FFD-27E2-448A-9448-57D9C2126E28}"/>
+    <hyperlink ref="E251" r:id="rId38" xr:uid="{A71649C1-DFA1-47F0-A83A-DD46B1D9F33B}"/>
+    <hyperlink ref="E252" r:id="rId39" xr:uid="{FAB07CFA-C42D-41C3-BC51-6C047A4F631A}"/>
+    <hyperlink ref="E253" r:id="rId40" xr:uid="{07619AD0-FAE6-435B-933F-CADCBCFB7840}"/>
+    <hyperlink ref="E254" r:id="rId41" xr:uid="{BF836E66-ACE5-4E9F-A1D5-374BB72BE8CD}"/>
+    <hyperlink ref="E255" r:id="rId42" xr:uid="{E8CDD1A1-3121-4285-B763-61A156B33C5B}"/>
+    <hyperlink ref="E256" r:id="rId43" xr:uid="{EDC00FDA-9338-4D77-B6C2-9633EAE3400C}"/>
+    <hyperlink ref="E257" r:id="rId44" xr:uid="{6242D261-0408-422E-85E1-5A1059452DB6}"/>
+    <hyperlink ref="E259" r:id="rId45" xr:uid="{F1AD0927-7EB5-4CC5-BBDD-86587215D0BB}"/>
+    <hyperlink ref="E260" r:id="rId46" xr:uid="{A847F8EA-73B5-49F7-901D-7F0DF51072A2}"/>
+    <hyperlink ref="E261" r:id="rId47" xr:uid="{D99B0E47-2B79-4B99-80FE-5F958BC7663A}"/>
+    <hyperlink ref="E262" r:id="rId48" xr:uid="{CE0539A5-9647-4DC2-9434-960FC3133125}"/>
+    <hyperlink ref="E263" r:id="rId49" xr:uid="{EAE0914A-0E47-4E80-A9F3-CD31D380793A}"/>
+    <hyperlink ref="E264" r:id="rId50" xr:uid="{153CA75C-A630-4B0D-A906-9E733A202349}"/>
+    <hyperlink ref="E265" r:id="rId51" xr:uid="{0F0FC67D-5F22-487B-81C4-66A4EBC83AC0}"/>
+    <hyperlink ref="E266" r:id="rId52" xr:uid="{7B4CBFA4-0378-4C60-811E-E851B2E6596B}"/>
+    <hyperlink ref="E267" r:id="rId53" xr:uid="{9D2AB88A-F8B2-405C-B078-D58E56BE7F87}"/>
+    <hyperlink ref="E268" r:id="rId54" xr:uid="{A3C3338B-E99C-49AB-90E1-71BD9E2301AE}"/>
+    <hyperlink ref="E269" r:id="rId55" xr:uid="{FAAA03F7-583A-4CBC-A50D-B45C8192A0A2}"/>
+    <hyperlink ref="E273" r:id="rId56" xr:uid="{69F0DE51-5E60-43FF-96AF-598BE7584449}"/>
+    <hyperlink ref="E275" r:id="rId57" xr:uid="{F2989BFE-F40E-4508-A142-140AE28EFD15}"/>
+    <hyperlink ref="E276" r:id="rId58" xr:uid="{876B1468-4D68-4C90-95EC-0608E44F7790}"/>
+    <hyperlink ref="E277" r:id="rId59" xr:uid="{737800C7-6399-4507-923E-904795C2796C}"/>
+    <hyperlink ref="E278" r:id="rId60" xr:uid="{23CA6B86-1AB4-49F3-8AD9-A2DBB2386443}"/>
+    <hyperlink ref="E279" r:id="rId61" xr:uid="{CCC6603D-C50B-4D55-84D3-7706BA4DC8D4}"/>
+    <hyperlink ref="E280" r:id="rId62" xr:uid="{7CD86F1D-73E2-4227-A288-1AFB610A4AAD}"/>
+    <hyperlink ref="E281" r:id="rId63" xr:uid="{984AB3C0-939A-4F5F-9232-2A3586971B1B}"/>
+    <hyperlink ref="E282" r:id="rId64" xr:uid="{2B00815D-736D-47B3-BD98-3B0C8693DC05}"/>
+    <hyperlink ref="E283" r:id="rId65" xr:uid="{9DD1F895-0083-401D-BF30-DDC875420B67}"/>
+    <hyperlink ref="E284" r:id="rId66" xr:uid="{A9D5C317-BD82-4381-99EE-705F9EEE33BB}"/>
+    <hyperlink ref="E285" r:id="rId67" xr:uid="{3C8B2531-7964-4F9B-A70C-BB302C67E9C6}"/>
+    <hyperlink ref="E286" r:id="rId68" xr:uid="{B796C198-8ECF-4046-A532-BA3CB7F58EF0}"/>
+    <hyperlink ref="E287" r:id="rId69" xr:uid="{77E20E7E-73DC-48E6-901B-9D6E715AD0B4}"/>
+    <hyperlink ref="E288" r:id="rId70" xr:uid="{BB8BD08E-2A2A-49BD-9AAB-866984928F6E}"/>
+    <hyperlink ref="E289" r:id="rId71" xr:uid="{D4BD10D4-8EA0-4EDE-B05B-59BC68420806}"/>
+    <hyperlink ref="E290" r:id="rId72" xr:uid="{241C3D35-1723-4E4B-B14F-0C2E924F2EF7}"/>
+    <hyperlink ref="E291" r:id="rId73" xr:uid="{FEE28247-B6C4-48E8-820B-1C18EF2A652F}"/>
+    <hyperlink ref="E292" r:id="rId74" xr:uid="{D6B3C273-BAD1-48E9-A3B0-1E0816ADDFC9}"/>
+    <hyperlink ref="E293" r:id="rId75" xr:uid="{974C071F-49C0-4D49-969F-4ECB408ABFC7}"/>
+    <hyperlink ref="E294" r:id="rId76" xr:uid="{6E1683AD-2C5D-4637-9B2C-15157DFE3084}"/>
+    <hyperlink ref="E295" r:id="rId77" xr:uid="{0696468C-0321-42E0-9220-47E31D0D9E6F}"/>
+    <hyperlink ref="E296" r:id="rId78" xr:uid="{207D43E8-43D3-45EF-BD8E-EEA4A3B35166}"/>
+    <hyperlink ref="E297" r:id="rId79" xr:uid="{A3F3DF2C-BBF6-4640-9EA3-3E46C4DBA999}"/>
+    <hyperlink ref="E298" r:id="rId80" xr:uid="{A1144EE1-CC15-4034-9088-ED7584043E12}"/>
+    <hyperlink ref="E299" r:id="rId81" xr:uid="{B181A9F5-7C4E-4376-88D0-FC5BEF321929}"/>
+    <hyperlink ref="E300" r:id="rId82" xr:uid="{B1B20292-BB6A-4F7D-A3A2-96398457CA75}"/>
+    <hyperlink ref="E301" r:id="rId83" xr:uid="{3B9158DB-A206-4644-9F57-DBBA32AD5385}"/>
+    <hyperlink ref="E302" r:id="rId84" xr:uid="{B7909C77-0FDB-4DC4-9623-7FE022D71678}"/>
+    <hyperlink ref="E304" r:id="rId85" xr:uid="{DC604A37-A995-4640-B7B3-B4C3DAF1484E}"/>
+    <hyperlink ref="E305" r:id="rId86" xr:uid="{9B9A155E-60BB-4642-8E56-077E4A816907}"/>
+    <hyperlink ref="E306" r:id="rId87" xr:uid="{F61E495A-793D-4A15-813A-F8248A2EA9FC}"/>
+    <hyperlink ref="E307" r:id="rId88" xr:uid="{B580676C-F2A9-4149-9E3A-1CE15BDC56EA}"/>
+    <hyperlink ref="E308" r:id="rId89" xr:uid="{1978FC6A-A4FC-4A32-AAE3-4461A1526402}"/>
+    <hyperlink ref="E309" r:id="rId90" xr:uid="{34E686AB-EB45-4140-B868-D707DE4B9CD3}"/>
+    <hyperlink ref="E310" r:id="rId91" xr:uid="{30E623A0-8328-49C5-A754-CFEF4DC03EE5}"/>
+    <hyperlink ref="E311" r:id="rId92" xr:uid="{B920584A-746B-4CB8-8989-257CFD744010}"/>
+    <hyperlink ref="E313" r:id="rId93" xr:uid="{03510B87-AD63-4CBE-85D7-52EFF5081E13}"/>
+    <hyperlink ref="E314" r:id="rId94" xr:uid="{70B78D94-4DB9-4176-968E-BA5D3CC97EEA}"/>
+    <hyperlink ref="E315" r:id="rId95" xr:uid="{28BFE190-590E-4BDB-BA27-5F8149A471DD}"/>
+    <hyperlink ref="E316" r:id="rId96" xr:uid="{D91A404F-35E1-49F6-96A4-3C3848A80A2A}"/>
+    <hyperlink ref="E317" r:id="rId97" xr:uid="{B2BC2FC6-0C1F-4AC2-B771-D75F1796771C}"/>
+    <hyperlink ref="E318" r:id="rId98" xr:uid="{467180E5-64CE-4968-8668-306140491CCE}"/>
+    <hyperlink ref="E319" r:id="rId99" xr:uid="{540CFE43-14AC-45E6-B344-0487A5EEFBE1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>